<commit_message>
Data catalogue for considerations
</commit_message>
<xml_diff>
--- a/data_catalogue.xlsx
+++ b/data_catalogue.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bpfree/Documents/HUB Ocean/Projects/Total Energies/north-sea_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5643B0C4-7B5C-F143-91D7-4BA56377E18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACF6FD5-6342-784C-8F28-C58A61BE7A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="56300" yWindow="6920" windowWidth="28040" windowHeight="17180" xr2:uid="{D45F491C-9D82-D841-81AB-10163D37C38A}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" xr2:uid="{D45F491C-9D82-D841-81AB-10163D37C38A}"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="1" r:id="rId1"/>
     <sheet name="Future" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="135">
   <si>
     <t>Domain</t>
   </si>
@@ -385,6 +385,63 @@
   </si>
   <si>
     <t>https://app.hubocean.earth/catalog/dataset/019be45f-154f-4b48-ab01-651b237ab1d9/global-whale-distribution-ship-strike-risk-and-hotspots-nisi-et-al-2024-</t>
+  </si>
+  <si>
+    <t>WCMC</t>
+  </si>
+  <si>
+    <t>ODP</t>
+  </si>
+  <si>
+    <t>7199f9bc-96ae-49d1-a814-df8c4bcc7552</t>
+  </si>
+  <si>
+    <t>Visualization</t>
+  </si>
+  <si>
+    <t>No use for commercial?</t>
+  </si>
+  <si>
+    <t>Basically none in the study region (out of date)</t>
+  </si>
+  <si>
+    <t>Balogh et al. 2023</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S2352340923003426</t>
+  </si>
+  <si>
+    <t>WRI</t>
+  </si>
+  <si>
+    <t>Raster file</t>
+  </si>
+  <si>
+    <t>Exclude</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Maybe</t>
+  </si>
+  <si>
+    <t>Too large</t>
+  </si>
+  <si>
+    <t>Macroendobenthos presence / absence events</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Too coastal</t>
+  </si>
+  <si>
+    <t>https://emodnet.ec.europa.eu/geonetwork/srv/eng/catalog.search#/metadata/39746d9c-4220-425c-bc26-7cb3056c36a5</t>
+  </si>
+  <si>
+    <t>No use for commercial</t>
   </si>
 </sst>
 </file>
@@ -775,19 +832,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{369D950F-74A8-F94F-A561-0B69EA5AA7C4}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="59.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -810,13 +868,19 @@
         <v>9</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -832,11 +896,14 @@
       <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>127</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -852,8 +919,11 @@
       <c r="G3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -866,11 +936,14 @@
       <c r="G4" t="s">
         <v>10</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>127</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -883,348 +956,534 @@
       <c r="G5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
+      <c r="C6" t="s">
+        <v>126</v>
+      </c>
       <c r="G6" t="s">
         <v>16</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
+      <c r="C7" t="s">
+        <v>126</v>
+      </c>
       <c r="G7" t="s">
         <v>28</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
       <c r="G8" t="s">
         <v>11</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
+      <c r="C9" t="s">
+        <v>62</v>
+      </c>
       <c r="G9" t="s">
         <v>17</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="H10" t="s">
+      <c r="C10" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" t="s">
+        <v>124</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F11" t="s">
+        <v>128</v>
+      </c>
+      <c r="G11" t="s">
+        <v>122</v>
+      </c>
+      <c r="J11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="K13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="H12" t="s">
+      <c r="C14" t="s">
+        <v>126</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="I12" t="s">
+      <c r="K14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>33</v>
       </c>
-      <c r="H13" t="s">
+      <c r="C15" t="s">
+        <v>126</v>
+      </c>
+      <c r="J15" t="s">
         <v>80</v>
       </c>
-      <c r="I13" t="s">
+      <c r="K15" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>52</v>
       </c>
-      <c r="H14" t="s">
+      <c r="C16" t="s">
+        <v>131</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I14" t="s">
+      <c r="K16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>55</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>8</v>
       </c>
       <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
+        <v>131</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" t="s">
+        <v>126</v>
+      </c>
+      <c r="F18" t="s">
+        <v>127</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
         <v>50</v>
       </c>
-      <c r="H17" t="s">
+      <c r="C19" t="s">
+        <v>126</v>
+      </c>
+      <c r="F19" t="s">
+        <v>127</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" t="s">
-        <v>61</v>
-      </c>
-      <c r="H18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" t="s">
-        <v>67</v>
-      </c>
-      <c r="G19" t="s">
-        <v>65</v>
-      </c>
-      <c r="H19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>14</v>
       </c>
       <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
+        <v>126</v>
+      </c>
+      <c r="F20" t="s">
+        <v>127</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>126</v>
+      </c>
+      <c r="F21" t="s">
+        <v>127</v>
+      </c>
+      <c r="G21" t="s">
+        <v>65</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
         <v>68</v>
       </c>
-      <c r="G20" t="s">
+      <c r="C22" t="s">
+        <v>131</v>
+      </c>
+      <c r="G22" t="s">
         <v>69</v>
       </c>
-      <c r="H20" t="s">
+      <c r="J22" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="K22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>32</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>59</v>
       </c>
-      <c r="G21" t="s">
-        <v>65</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="C23" t="s">
+        <v>126</v>
+      </c>
+      <c r="G23" t="s">
+        <v>65</v>
+      </c>
+      <c r="J23" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>8</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>72</v>
       </c>
-      <c r="G22" t="s">
-        <v>65</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="C24" t="s">
+        <v>126</v>
+      </c>
+      <c r="G24" t="s">
+        <v>65</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" t="s">
-        <v>74</v>
-      </c>
-      <c r="G23" t="s">
-        <v>65</v>
-      </c>
-      <c r="H23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" t="s">
-        <v>81</v>
-      </c>
-      <c r="G24" t="s">
-        <v>65</v>
-      </c>
-      <c r="H24" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>8</v>
       </c>
       <c r="B25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25" t="s">
+        <v>65</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" t="s">
+        <v>65</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
         <v>83</v>
       </c>
-      <c r="G25" t="s">
-        <v>65</v>
-      </c>
-      <c r="H25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" t="s">
-        <v>84</v>
-      </c>
-      <c r="G26" t="s">
-        <v>65</v>
-      </c>
-      <c r="H26" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" t="s">
-        <v>86</v>
-      </c>
       <c r="G27" t="s">
         <v>65</v>
       </c>
-      <c r="H27" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>113</v>
+        <v>84</v>
+      </c>
+      <c r="C28" t="s">
+        <v>126</v>
       </c>
       <c r="G28" t="s">
-        <v>110</v>
-      </c>
-      <c r="H28" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K28" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>86</v>
+      </c>
+      <c r="C29" t="s">
+        <v>62</v>
       </c>
       <c r="G29" t="s">
-        <v>111</v>
-      </c>
-      <c r="H29" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="I29" t="s">
+        <v>127</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>8</v>
       </c>
       <c r="B30" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" t="s">
+        <v>126</v>
+      </c>
+      <c r="F30" t="s">
+        <v>128</v>
+      </c>
+      <c r="G30" t="s">
+        <v>110</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K30" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" t="s">
+        <v>126</v>
+      </c>
+      <c r="F31" t="s">
+        <v>128</v>
+      </c>
+      <c r="G31" t="s">
+        <v>111</v>
+      </c>
+      <c r="J31" t="s">
+        <v>112</v>
+      </c>
+      <c r="K31" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
         <v>114</v>
       </c>
-      <c r="H30" t="s">
+      <c r="C32" t="s">
+        <v>126</v>
+      </c>
+      <c r="F32" t="s">
+        <v>128</v>
+      </c>
+      <c r="J32" t="s">
         <v>115</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H15" r:id="rId1" xr:uid="{1B1CB6C7-3768-F046-81D9-7675AEDF6FC6}"/>
+    <hyperlink ref="J17" r:id="rId1" xr:uid="{1B1CB6C7-3768-F046-81D9-7675AEDF6FC6}"/>
+    <hyperlink ref="J16" r:id="rId2" xr:uid="{D6AD33BF-B7A4-364D-B356-25A4338ADC01}"/>
+    <hyperlink ref="J2" r:id="rId3" xr:uid="{6A37A3BD-FB4E-074D-98C1-F2618E74E02A}"/>
+    <hyperlink ref="J4" r:id="rId4" xr:uid="{883A5C53-E1EF-894E-B9A5-0F39424C9A9B}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{851675A5-31F7-0B46-9F7B-D76A2F45E8C8}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{0FAECF2A-81BA-F542-8A12-0C7F09FE6B9E}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{C4021B33-3E9F-344A-A9C0-51CBA2C59F7A}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{ECD9122A-1AA1-604B-91C2-3BD62395BB61}"/>
+    <hyperlink ref="J10" r:id="rId9" display="https://resourcewatch.org/data/explore/bio033-Cold-Water-Corals_replacement?section=Discover&amp;selectedCollection=&amp;zoom=4.072722144183686&amp;lat=53.43196080481361&amp;lng=10.90726865654836&amp;pitch=0&amp;bearing=0&amp;basemap=dark&amp;labels=light&amp;layers=%255B%257B%2522dataset%2522%253A%25221bc94710-d7ec-46f9-aa27-edddd87b1625%2522%252C%2522opacity%2522%253A1%252C%2522layer%2522%253A%2522eacf9f96-228d-4492-8998-ec1d873927aa%2522%257D%255D&amp;aoi=&amp;page=1&amp;sort=most-viewed&amp;sortDirection=-1" xr:uid="{7FE2EF65-23A1-BC4D-8178-8F929496D4AF}"/>
+    <hyperlink ref="J14" r:id="rId10" xr:uid="{6C8956F0-177D-C443-8CD3-AD4B14557AFF}"/>
+    <hyperlink ref="J18" r:id="rId11" xr:uid="{87A41796-9193-2A41-9F55-D4D09AAD15F5}"/>
+    <hyperlink ref="J19" r:id="rId12" xr:uid="{8D123B17-70AC-D342-A3C9-6DF99EF31E46}"/>
+    <hyperlink ref="J20" r:id="rId13" xr:uid="{EC17493E-17A9-2F4F-9260-047D4143563B}"/>
+    <hyperlink ref="J21" r:id="rId14" location="/metadata/6d617269-6e65-696e-666f-000000008730" xr:uid="{F1C96E57-B5BB-7E43-BBAF-B102597202DC}"/>
+    <hyperlink ref="J22" r:id="rId15" location="/metadata/6d617269-6e65-696e-666f-000000001510" xr:uid="{FF3095AF-1320-6E47-B6ED-7B6251EA8828}"/>
+    <hyperlink ref="J23" r:id="rId16" xr:uid="{C0E0C20F-A2AB-594A-BB98-8A09F517114A}"/>
+    <hyperlink ref="J24" r:id="rId17" location="/metadata/6d617269-6e65-696e-666f-000000008216" xr:uid="{2AECCFA5-01FF-ED4A-8366-006157BBBB49}"/>
+    <hyperlink ref="J25" r:id="rId18" location="/metadata/6d617269-6e65-696e-666f-000000006648" xr:uid="{01D2178B-73B0-504F-B3B7-CE8BE361194D}"/>
+    <hyperlink ref="J26" r:id="rId19" location="/metadata/6d617269-6e65-696e-666f-000000008777" xr:uid="{646F8C9B-D6D3-8043-A64C-6CE3235228AB}"/>
+    <hyperlink ref="J28" r:id="rId20" location="/metadata/6d617269-6e65-696e-666f-000000008820" xr:uid="{D8801DF4-8FB4-2E4D-B672-4B88E1F3F1C1}"/>
+    <hyperlink ref="J29" r:id="rId21" location="/metadata/6d617269-6e65-696e-666f-000000008880" xr:uid="{9763DFB9-A41C-8E4C-927B-0671C801FC61}"/>
+    <hyperlink ref="J30" r:id="rId22" xr:uid="{4E5DEB25-A974-7244-BF87-C738FD3D47E7}"/>
+    <hyperlink ref="J13" r:id="rId23" location="/metadata/39746d9c-4220-425c-bc26-7cb3056c36a5" xr:uid="{1F777F7B-0DB3-AE4F-B869-952743B7CDCC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1232,10 +1491,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9069362E-F3BD-1B45-8F6F-44A5A27E3ED2}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1539,7 +1798,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>63</v>
       </c>
@@ -1550,9 +1809,23 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
+        <v>130</v>
+      </c>
+      <c r="G37" t="s">
+        <v>65</v>
+      </c>
+      <c r="H37" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>